<commit_message>
updated daily scrum journal and sprint task sheet
</commit_message>
<xml_diff>
--- a/Agile Documentation/DAILY SCRUM SHEET.xlsx
+++ b/Agile Documentation/DAILY SCRUM SHEET.xlsx
@@ -11,15 +11,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Stand-up questions</t>
   </si>
   <si>
-    <t xml:space="preserve">Week 1 # </t>
+    <t xml:space="preserve">Week #1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week #2 </t>
   </si>
   <si>
     <t>10/8/2021 - 10/15/2021</t>
+  </si>
+  <si>
+    <t>10/16/2021 - 10/22/2021</t>
   </si>
   <si>
     <t>ISHA</t>
@@ -33,10 +39,16 @@
 flight booking functionality</t>
   </si>
   <si>
+    <t>Devloped UI wireframes for my trips and cancel/update flight screen, developed UI for home page of airline website</t>
+  </si>
+  <si>
     <t>What am I planning to work on next?</t>
   </si>
   <si>
     <t>develop the home page for airline system</t>
+  </si>
+  <si>
+    <t>developing functionalities for airline</t>
   </si>
   <si>
     <t>What tasks are blocked waiting on another team member?</t>
@@ -58,7 +70,11 @@
 with the relationship</t>
   </si>
   <si>
-    <t>Table creation and DB design</t>
+    <t>Understanding flow of mileage plus account,
+DB Design and table creation, mock data for all tables and UI wireframe for login and traveller details page</t>
+  </si>
+  <si>
+    <t>Table creation and DB design,mock data for all tables</t>
   </si>
   <si>
     <t>Through regular meetings, everyone received constant constructive feedback which help us achieved the well reviewed solution</t>
@@ -70,10 +86,16 @@
     <t>Architecture diagram ,UI wireframe for customer signup and Home</t>
   </si>
   <si>
+    <t>Design and creation of tables namely Booking, Seat, FlightSeat, Traveller in DB and review with the team. Created UI wireframe for Mileage details page</t>
+  </si>
+  <si>
     <t>DB design</t>
   </si>
   <si>
     <t>Communication - Discussion about technology stack and requirements</t>
+  </si>
+  <si>
+    <t>Communication, feedback -Discussed about the design decisions with the team and got it reviewed.</t>
   </si>
   <si>
     <t>ANIL</t>
@@ -82,10 +104,19 @@
     <t>Project setup &amp; boilerplate code</t>
   </si>
   <si>
+    <t xml:space="preserve">Integrated mysql , sign in page mock. </t>
+  </si>
+  <si>
     <t>Integrate Mysql &amp; mock login page</t>
   </si>
   <si>
-    <t>Respect - discuss others choices of design</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Respect - others choice of design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication - DB design discussions. </t>
   </si>
 </sst>
 </file>
@@ -95,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -110,6 +141,9 @@
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
     </font>
     <font>
       <b/>
@@ -188,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -221,7 +255,13 @@
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -445,6 +485,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="81.0"/>
     <col customWidth="1" min="2" max="2" width="41.86"/>
+    <col customWidth="1" min="3" max="3" width="39.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -454,7 +495,9 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -481,9 +524,11 @@
     <row r="2">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -509,7 +554,7 @@
     </row>
     <row r="3" ht="30.0" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -538,12 +583,14 @@
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -569,12 +616,14 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>7</v>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -600,12 +649,14 @@
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -630,13 +681,12 @@
       <c r="Y6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
-        <v>10</v>
+      <c r="A7" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
+      <c r="B7" s="15" t="s">
+        <v>15</v>
       </c>
-      <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -662,10 +712,8 @@
     </row>
     <row r="8" ht="30.0" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -691,12 +739,14 @@
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -722,10 +772,10 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>14</v>
+      <c r="B10" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -753,12 +803,14 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -783,13 +835,12 @@
       <c r="Y11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
-        <v>10</v>
+      <c r="A12" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>15</v>
+      <c r="B12" s="15" t="s">
+        <v>20</v>
       </c>
-      <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -815,7 +866,7 @@
     </row>
     <row r="13" ht="30.0" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -844,12 +895,14 @@
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>17</v>
+      <c r="B14" s="15" t="s">
+        <v>22</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -875,10 +928,10 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>18</v>
+      <c r="B15" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -906,12 +959,14 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -936,13 +991,15 @@
       <c r="Y16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>10</v>
+      <c r="A17" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>19</v>
+      <c r="B17" s="12" t="s">
+        <v>25</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -968,7 +1025,7 @@
     </row>
     <row r="18" ht="30.0" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -997,12 +1054,14 @@
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -1028,10 +1087,10 @@
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1059,12 +1118,14 @@
     </row>
     <row r="21">
       <c r="A21" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>9</v>
+      <c r="B21" s="13" t="s">
+        <v>13</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1089,13 +1150,15 @@
       <c r="Y21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="s">
-        <v>10</v>
+      <c r="A22" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>23</v>
+      <c r="B22" s="12" t="s">
+        <v>32</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -27580,6 +27643,10 @@
       <c r="Y1002" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Booking changes and sprint sheets
</commit_message>
<xml_diff>
--- a/Agile Documentation/DAILY SCRUM SHEET.xlsx
+++ b/Agile Documentation/DAILY SCRUM SHEET.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Stand-up questions</t>
   </si>
@@ -22,10 +22,22 @@
     <t xml:space="preserve">Week #2 </t>
   </si>
   <si>
+    <t>Week #3</t>
+  </si>
+  <si>
+    <t>Week #4</t>
+  </si>
+  <si>
     <t>10/8/2021 - 10/15/2021</t>
   </si>
   <si>
     <t>10/16/2021 - 10/22/2021</t>
+  </si>
+  <si>
+    <t>10/22/2021 - 10/28/2021</t>
+  </si>
+  <si>
+    <t>10/28/2021 - 11/04/2021</t>
   </si>
   <si>
     <t>ISHA</t>
@@ -42,6 +54,9 @@
     <t>Devloped UI wireframes for my trips and cancel/update flight screen, developed UI for home page of airline website</t>
   </si>
   <si>
+    <t xml:space="preserve">developed the front end for flight booking screen </t>
+  </si>
+  <si>
     <t>What am I planning to work on next?</t>
   </si>
   <si>
@@ -49,6 +64,9 @@
   </si>
   <si>
     <t>developing functionalities for airline</t>
+  </si>
+  <si>
+    <t>developing the flight listing screen for the website</t>
   </si>
   <si>
     <t>What tasks are blocked waiting on another team member?</t>
@@ -60,7 +78,7 @@
     <t>Select one of the XP Core Values and keep a journal of how the team kept these values throughout the project.</t>
   </si>
   <si>
-    <t xml:space="preserve">we discussed our task progress in the daily meeting and solved any blockers we faced together </t>
+    <t>we discussed our task progress in the daily meeting and solved any blockers we faced together (XP value: communication)</t>
   </si>
   <si>
     <t>HIMAKSHI</t>
@@ -74,10 +92,25 @@
 DB Design and table creation, mock data for all tables and UI wireframe for login and traveller details page</t>
   </si>
   <si>
+    <t>Developed Booking history page frontend and backend</t>
+  </si>
+  <si>
+    <t>Developed Cancel booking option frontend</t>
+  </si>
+  <si>
     <t>Table creation and DB design,mock data for all tables</t>
   </si>
   <si>
-    <t>Through regular meetings, everyone received constant constructive feedback which help us achieved the well reviewed solution</t>
+    <t>Booking history pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developing Cancel booking option </t>
+  </si>
+  <si>
+    <t>Developing Cancel and Edit booking option frontend and backend</t>
+  </si>
+  <si>
+    <t>Through regular meetings, everyone discussed functionalities in details which help us achieved the well reviewed solution.</t>
   </si>
   <si>
     <t>JAHNAVI</t>
@@ -89,13 +122,25 @@
     <t>Design and creation of tables namely Booking, Seat, FlightSeat, Traveller in DB and review with the team. Created UI wireframe for Mileage details page</t>
   </si>
   <si>
+    <t>Designed and implemented Login and signup pages on both frontend and backend</t>
+  </si>
+  <si>
     <t>DB design</t>
+  </si>
+  <si>
+    <t>Signin and Signup pages</t>
+  </si>
+  <si>
+    <t>Mileage rewards account page</t>
   </si>
   <si>
     <t>Communication - Discussion about technology stack and requirements</t>
   </si>
   <si>
-    <t>Communication, feedback -Discussed about the design decisions with the team and got it reviewed.</t>
+    <t>Communication - Discussed about the design decisions with the team and got it reviewed.</t>
+  </si>
+  <si>
+    <t>Communication - Effectively communicated with the team related toapproach and implementation</t>
   </si>
   <si>
     <t>ANIL</t>
@@ -107,7 +152,16 @@
     <t xml:space="preserve">Integrated mysql , sign in page mock. </t>
   </si>
   <si>
+    <t>Created basic seat map with seat numbers</t>
+  </si>
+  <si>
     <t>Integrate Mysql &amp; mock login page</t>
+  </si>
+  <si>
+    <t>Design Seat booking UI</t>
+  </si>
+  <si>
+    <t>Integrate backed and update seat details dynamically</t>
   </si>
   <si>
     <t>None</t>
@@ -117,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">Communication - DB design discussions. </t>
+  </si>
+  <si>
+    <t>Communication - discussed seat map design for seat selection</t>
   </si>
 </sst>
 </file>
@@ -143,13 +200,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-    </font>
-    <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="&quot;Trebuchet MS&quot;"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -222,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -255,17 +312,14 @@
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,6 +540,8 @@
     <col customWidth="1" min="1" max="1" width="81.0"/>
     <col customWidth="1" min="2" max="2" width="41.86"/>
     <col customWidth="1" min="3" max="3" width="39.86"/>
+    <col customWidth="1" min="4" max="4" width="54.43"/>
+    <col customWidth="1" min="5" max="5" width="32.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,8 +554,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -524,13 +584,17 @@
     <row r="2">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -554,7 +618,7 @@
     </row>
     <row r="3" ht="30.0" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -583,15 +647,17 @@
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -616,15 +682,17 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>10</v>
+      <c r="B5" s="10" t="s">
+        <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>11</v>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -649,15 +717,17 @@
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>13</v>
+      <c r="C6" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -681,13 +751,12 @@
       <c r="Y6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
-        <v>14</v>
+      <c r="A7" s="13" t="s">
+        <v>20</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>15</v>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
       </c>
-      <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -712,7 +781,7 @@
     </row>
     <row r="8" ht="30.0" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -739,16 +808,20 @@
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>18</v>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -772,14 +845,20 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>19</v>
+      <c r="B10" s="10" t="s">
+        <v>27</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -803,16 +882,20 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>13</v>
+      <c r="C11" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -835,14 +918,12 @@
       <c r="Y11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="B12" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -866,7 +947,7 @@
     </row>
     <row r="13" ht="30.0" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -895,15 +976,17 @@
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>22</v>
+      <c r="B14" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -928,13 +1011,17 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>24</v>
+      <c r="B15" s="10" t="s">
+        <v>36</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="C15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -959,15 +1046,17 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>13</v>
+      <c r="C16" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -991,16 +1080,18 @@
       <c r="Y16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="14" t="s">
-        <v>14</v>
+      <c r="A17" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -1025,7 +1116,7 @@
     </row>
     <row r="18" ht="30.0" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1054,15 +1145,17 @@
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>29</v>
+      <c r="C19" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1087,13 +1180,17 @@
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="C20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -1118,15 +1215,17 @@
     </row>
     <row r="21">
       <c r="A21" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>13</v>
+      <c r="B21" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>31</v>
+      <c r="C21" s="10" t="s">
+        <v>49</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1150,16 +1249,18 @@
       <c r="Y21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="14" t="s">
-        <v>14</v>
+      <c r="A22" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>33</v>
+      <c r="C22" s="10" t="s">
+        <v>51</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -27644,8 +27745,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B12:E12"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>